<commit_message>
Add user list for admin.
Add users view and model to the admin frontend.

Add user list page.
</commit_message>
<xml_diff>
--- a/src/main/dictionary/Exercises.xlsx
+++ b/src/main/dictionary/Exercises.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="121">
   <si>
     <t>id</t>
   </si>
@@ -22,10 +22,7 @@
     <t>Norwegian</t>
   </si>
   <si>
-    <t>Criteria list</t>
-  </si>
-  <si>
-    <t>Criteria list examples</t>
+    <t>Exercise type</t>
   </si>
   <si>
     <t>Legs</t>
@@ -40,10 +37,7 @@
     <t>Knebøy</t>
   </si>
   <si>
-    <t>Set, Repetitions,Weight</t>
-  </si>
-  <si>
-    <t>1, 5, 10</t>
+    <t>strenght</t>
   </si>
   <si>
     <t>Front Squat</t>
@@ -505,7 +499,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -514,7 +508,7 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -526,7 +520,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1639,7 +1633,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1647,11 +1641,10 @@
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.5781" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6562" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.0469" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7344" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7344" style="1" customWidth="1"/>
-    <col min="7" max="256" width="10.7344" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7344" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.9062" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.2266" style="1" customWidth="1"/>
+    <col min="6" max="256" width="10.7344" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17" customHeight="1">
@@ -1667,769 +1660,796 @@
       <c r="D1" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="17" customHeight="1">
       <c r="A2" s="5">
         <v>10</v>
       </c>
       <c r="B2" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s" s="6">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="6">
-        <v>6</v>
-      </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="17" customHeight="1">
       <c r="A3" s="5">
         <v>20</v>
       </c>
       <c r="B3" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s" s="8">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="8">
-        <v>8</v>
-      </c>
       <c r="D3" t="s" s="3">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s" s="3">
-        <v>10</v>
-      </c>
-      <c r="F3" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="17" customHeight="1">
       <c r="A4" s="5">
         <v>30</v>
       </c>
       <c r="B4" t="s" s="3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s" s="8">
-        <v>12</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="D4" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="17" customHeight="1">
       <c r="A5" s="5">
         <v>40</v>
       </c>
       <c r="B5" t="s" s="3">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s" s="8">
-        <v>14</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="7"/>
+        <v>12</v>
+      </c>
+      <c r="D5" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="17" customHeight="1">
       <c r="A6" s="5">
         <v>50</v>
       </c>
       <c r="B6" t="s" s="3">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s" s="8">
-        <v>16</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="D6" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="17" customHeight="1">
       <c r="A7" s="5">
         <v>60</v>
       </c>
       <c r="B7" t="s" s="3">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="7"/>
+        <v>16</v>
+      </c>
+      <c r="D7" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="17" customHeight="1">
       <c r="A8" s="5">
         <v>70</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s" s="9">
-        <v>20</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="7"/>
+        <v>18</v>
+      </c>
+      <c r="D8" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="17" customHeight="1">
       <c r="A9" s="5">
         <v>80</v>
       </c>
       <c r="B9" t="s" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="D9" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="17" customHeight="1">
       <c r="A10" s="5">
         <v>90</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s" s="10">
-        <v>23</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="D10" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" ht="17" customHeight="1">
       <c r="A11" s="5">
         <v>100</v>
       </c>
       <c r="B11" t="s" s="3">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="D11" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" ht="17" customHeight="1">
       <c r="A12" s="5">
         <v>110</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s" s="3">
-        <v>27</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="D12" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" ht="17" customHeight="1">
       <c r="A13" s="5">
         <v>120</v>
       </c>
       <c r="B13" t="s" s="3">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s" s="3">
-        <v>29</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="D13" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" ht="17" customHeight="1">
       <c r="A14" s="5">
         <v>130</v>
       </c>
       <c r="B14" t="s" s="3">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s" s="3">
-        <v>31</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="7"/>
+        <v>29</v>
+      </c>
+      <c r="D14" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" ht="17" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="7"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" ht="17" customHeight="1">
       <c r="A16" s="5">
         <v>140</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="7"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" ht="17" customHeight="1">
       <c r="A17" s="5">
         <v>150</v>
       </c>
       <c r="B17" t="s" s="3">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s" s="3">
-        <v>34</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="D17" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" ht="17" customHeight="1">
       <c r="A18" s="5">
         <v>160</v>
       </c>
       <c r="B18" t="s" s="3">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s" s="3">
-        <v>35</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="D18" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" ht="17" customHeight="1">
       <c r="A19" s="5">
         <v>170</v>
       </c>
       <c r="B19" t="s" s="3">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s" s="3">
-        <v>37</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="7"/>
+        <v>35</v>
+      </c>
+      <c r="D19" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" ht="17" customHeight="1">
       <c r="A20" s="5">
         <v>180</v>
       </c>
       <c r="B20" t="s" s="3">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s" s="3">
-        <v>39</v>
-      </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="7"/>
+        <v>37</v>
+      </c>
+      <c r="D20" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" ht="17" customHeight="1">
       <c r="A21" s="5">
         <v>190</v>
       </c>
       <c r="B21" t="s" s="3">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s" s="3">
-        <v>41</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="D21" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" ht="17" customHeight="1">
       <c r="A22" s="5">
         <v>200</v>
       </c>
       <c r="B22" t="s" s="3">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s" s="3">
-        <v>43</v>
-      </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="D22" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" ht="17" customHeight="1">
       <c r="A23" s="5">
         <v>210</v>
       </c>
       <c r="B23" t="s" s="3">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C23" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="7"/>
+        <v>12</v>
+      </c>
+      <c r="D23" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" ht="17" customHeight="1">
       <c r="A24" s="5">
         <v>220</v>
       </c>
       <c r="B24" t="s" s="3">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s" s="3">
-        <v>27</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="D24" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" ht="17" customHeight="1">
       <c r="A25" s="5">
         <v>230</v>
       </c>
       <c r="B25" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s" s="3">
-        <v>45</v>
-      </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="D25" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E25" s="7"/>
     </row>
     <row r="26" ht="17" customHeight="1">
       <c r="A26" s="5">
         <v>240</v>
       </c>
       <c r="B26" t="s" s="3">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s" s="3">
-        <v>47</v>
-      </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="D26" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" ht="17" customHeight="1">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="7"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" ht="17" customHeight="1">
       <c r="A28" s="5">
         <v>250</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s" s="2">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="7"/>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" ht="17" customHeight="1">
       <c r="A29" s="5">
         <v>260</v>
       </c>
       <c r="B29" t="s" s="3">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s" s="3">
-        <v>51</v>
-      </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="7"/>
+        <v>49</v>
+      </c>
+      <c r="D29" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" ht="17" customHeight="1">
       <c r="A30" s="5">
         <v>270</v>
       </c>
       <c r="B30" t="s" s="3">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s" s="3">
-        <v>53</v>
-      </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="D30" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" ht="17" customHeight="1">
       <c r="A31" s="5">
         <v>280</v>
       </c>
       <c r="B31" t="s" s="3">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s" s="3">
-        <v>55</v>
-      </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="7"/>
+        <v>53</v>
+      </c>
+      <c r="D31" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" ht="17" customHeight="1">
       <c r="A32" s="5">
         <v>290</v>
       </c>
       <c r="B32" t="s" s="3">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C32" t="s" s="3">
-        <v>57</v>
-      </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="7"/>
+        <v>55</v>
+      </c>
+      <c r="D32" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E32" s="7"/>
     </row>
     <row r="33" ht="17" customHeight="1">
       <c r="A33" s="5">
         <v>300</v>
       </c>
       <c r="B33" t="s" s="3">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s" s="3">
-        <v>59</v>
-      </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="7"/>
+        <v>57</v>
+      </c>
+      <c r="D33" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" ht="17" customHeight="1">
       <c r="A34" s="5">
         <v>310</v>
       </c>
       <c r="B34" t="s" s="3">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s" s="3">
-        <v>61</v>
-      </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="7"/>
+        <v>59</v>
+      </c>
+      <c r="D34" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" ht="17" customHeight="1">
       <c r="A35" s="5">
         <v>320</v>
       </c>
       <c r="B35" t="s" s="3">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C35" t="s" s="3">
-        <v>63</v>
-      </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="7"/>
+        <v>61</v>
+      </c>
+      <c r="D35" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" ht="17" customHeight="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="7"/>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" ht="17" customHeight="1">
       <c r="A37" s="5">
         <v>330</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="7"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" ht="17" customHeight="1">
       <c r="A38" s="5">
         <v>340</v>
       </c>
       <c r="B38" t="s" s="3">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C38" t="s" s="3">
-        <v>67</v>
-      </c>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="7"/>
+        <v>65</v>
+      </c>
+      <c r="D38" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" ht="17" customHeight="1">
       <c r="A39" s="5">
         <v>350</v>
       </c>
       <c r="B39" t="s" s="3">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C39" t="s" s="3">
-        <v>69</v>
-      </c>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="7"/>
+        <v>67</v>
+      </c>
+      <c r="D39" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E39" s="7"/>
     </row>
     <row r="40" ht="17" customHeight="1">
       <c r="A40" s="5">
         <v>360</v>
       </c>
       <c r="B40" t="s" s="3">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C40" t="s" s="3">
-        <v>71</v>
-      </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="7"/>
+        <v>69</v>
+      </c>
+      <c r="D40" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" ht="17" customHeight="1">
       <c r="A41" s="5">
         <v>370</v>
       </c>
       <c r="B41" t="s" s="3">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C41" t="s" s="3">
-        <v>73</v>
-      </c>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="7"/>
+        <v>71</v>
+      </c>
+      <c r="D41" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" ht="17" customHeight="1">
       <c r="A42" s="5">
         <v>380</v>
       </c>
       <c r="B42" t="s" s="3">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C42" t="s" s="3">
-        <v>75</v>
-      </c>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="7"/>
+        <v>73</v>
+      </c>
+      <c r="D42" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E42" s="7"/>
     </row>
     <row r="43" ht="17" customHeight="1">
       <c r="A43" s="5">
         <v>390</v>
       </c>
       <c r="B43" t="s" s="3">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C43" t="s" s="3">
-        <v>77</v>
-      </c>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="D43" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E43" s="7"/>
     </row>
     <row r="44" ht="17" customHeight="1">
       <c r="A44" s="5">
         <v>400</v>
       </c>
       <c r="B44" t="s" s="3">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C44" t="s" s="3">
-        <v>79</v>
-      </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="7"/>
+        <v>77</v>
+      </c>
+      <c r="D44" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E44" s="7"/>
     </row>
     <row r="45" ht="17" customHeight="1">
       <c r="A45" s="5">
         <v>410</v>
       </c>
       <c r="B45" t="s" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C45" t="s" s="3">
-        <v>45</v>
-      </c>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="D45" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E45" s="7"/>
     </row>
     <row r="46" ht="17" customHeight="1">
       <c r="A46" s="5">
         <v>420</v>
       </c>
       <c r="B46" t="s" s="3">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C46" t="s" s="3">
-        <v>47</v>
-      </c>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="D46" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E46" s="7"/>
     </row>
     <row r="47" ht="17" customHeight="1">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="7"/>
+      <c r="E47" s="7"/>
     </row>
     <row r="48" ht="17" customHeight="1">
       <c r="A48" s="5">
         <v>430</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C48" t="s" s="2">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="7"/>
+      <c r="E48" s="7"/>
     </row>
     <row r="49" ht="17" customHeight="1">
       <c r="A49" s="5">
         <v>440</v>
       </c>
       <c r="B49" t="s" s="3">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C49" t="s" s="10">
-        <v>83</v>
-      </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="7"/>
+        <v>81</v>
+      </c>
+      <c r="D49" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E49" s="7"/>
     </row>
     <row r="50" ht="17" customHeight="1">
       <c r="A50" s="5">
         <v>450</v>
       </c>
       <c r="B50" t="s" s="3">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C50" t="s" s="8">
-        <v>85</v>
-      </c>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="7"/>
+        <v>83</v>
+      </c>
+      <c r="D50" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E50" s="7"/>
     </row>
     <row r="51" ht="17" customHeight="1">
       <c r="A51" s="5">
         <v>460</v>
       </c>
       <c r="B51" t="s" s="3">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C51" t="s" s="8">
-        <v>87</v>
-      </c>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="7"/>
+        <v>85</v>
+      </c>
+      <c r="D51" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E51" s="7"/>
     </row>
     <row r="52" ht="17" customHeight="1">
       <c r="A52" s="5">
         <v>470</v>
       </c>
       <c r="B52" t="s" s="3">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C52" t="s" s="8">
-        <v>89</v>
-      </c>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="7"/>
+        <v>87</v>
+      </c>
+      <c r="D52" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E52" s="7"/>
     </row>
     <row r="53" ht="17" customHeight="1">
       <c r="A53" s="5">
         <v>480</v>
       </c>
       <c r="B53" t="s" s="3">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C53" t="s" s="8">
-        <v>91</v>
-      </c>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="7"/>
+        <v>89</v>
+      </c>
+      <c r="D53" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E53" s="7"/>
     </row>
     <row r="54" ht="17" customHeight="1">
       <c r="A54" s="5">
         <v>490</v>
       </c>
       <c r="B54" t="s" s="3">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C54" t="s" s="9">
-        <v>93</v>
-      </c>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="7"/>
+        <v>91</v>
+      </c>
+      <c r="D54" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E54" s="7"/>
     </row>
     <row r="55" ht="17" customHeight="1">
       <c r="A55" s="5">
         <v>500</v>
       </c>
       <c r="B55" t="s" s="3">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C55" t="s" s="3">
-        <v>95</v>
-      </c>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="7"/>
+        <v>93</v>
+      </c>
+      <c r="D55" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E55" s="7"/>
     </row>
     <row r="56" ht="17" customHeight="1">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="7"/>
+      <c r="E56" s="7"/>
     </row>
     <row r="57" ht="17" customHeight="1">
       <c r="A57" s="5">
         <v>510</v>
       </c>
       <c r="B57" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="C57" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="D57" s="5"/>
+      <c r="E57" t="s" s="8">
         <v>96</v>
-      </c>
-      <c r="C57" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" t="s" s="8">
-        <v>98</v>
       </c>
     </row>
     <row r="58" ht="17" customHeight="1">
@@ -2437,212 +2457,220 @@
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="7"/>
+      <c r="E58" s="7"/>
     </row>
     <row r="59" ht="17" customHeight="1">
       <c r="A59" s="5">
         <v>520</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C59" t="s" s="2">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="7"/>
+      <c r="E59" s="7"/>
     </row>
     <row r="60" ht="17" customHeight="1">
       <c r="A60" s="5">
         <v>530</v>
       </c>
       <c r="B60" t="s" s="3">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C60" t="s" s="3">
-        <v>100</v>
-      </c>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="7"/>
+        <v>98</v>
+      </c>
+      <c r="D60" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E60" s="7"/>
     </row>
     <row r="61" ht="17" customHeight="1">
       <c r="A61" s="5">
         <v>540</v>
       </c>
       <c r="B61" t="s" s="3">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C61" t="s" s="3">
-        <v>102</v>
-      </c>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="7"/>
+        <v>100</v>
+      </c>
+      <c r="D61" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E61" s="7"/>
     </row>
     <row r="62" ht="17" customHeight="1">
       <c r="A62" s="5">
         <v>550</v>
       </c>
       <c r="B62" t="s" s="3">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C62" t="s" s="3">
-        <v>104</v>
-      </c>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="7"/>
+        <v>102</v>
+      </c>
+      <c r="D62" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E62" s="7"/>
     </row>
     <row r="63" ht="17" customHeight="1">
       <c r="A63" s="5">
         <v>560</v>
       </c>
       <c r="B63" t="s" s="3">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C63" t="s" s="3">
-        <v>106</v>
-      </c>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="7"/>
+        <v>104</v>
+      </c>
+      <c r="D63" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E63" s="7"/>
     </row>
     <row r="64" ht="17" customHeight="1">
       <c r="A64" s="5">
         <v>570</v>
       </c>
       <c r="B64" t="s" s="3">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C64" t="s" s="3">
-        <v>108</v>
-      </c>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="7"/>
+        <v>106</v>
+      </c>
+      <c r="D64" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E64" s="7"/>
     </row>
     <row r="65" ht="17" customHeight="1">
       <c r="A65" s="5">
         <v>580</v>
       </c>
       <c r="B65" t="s" s="3">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C65" t="s" s="3">
-        <v>110</v>
-      </c>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="7"/>
+        <v>108</v>
+      </c>
+      <c r="D65" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E65" s="7"/>
     </row>
     <row r="66" ht="17" customHeight="1">
       <c r="A66" s="5"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="7"/>
+      <c r="E66" s="7"/>
     </row>
     <row r="67" ht="17" customHeight="1">
       <c r="A67" s="5">
         <v>590</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C67" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="7"/>
+      <c r="E67" s="7"/>
     </row>
     <row r="68" ht="17" customHeight="1">
       <c r="A68" s="5">
         <v>600</v>
       </c>
       <c r="B68" t="s" s="3">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C68" t="s" s="3">
-        <v>113</v>
-      </c>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="7"/>
+        <v>111</v>
+      </c>
+      <c r="D68" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E68" s="7"/>
     </row>
     <row r="69" ht="17" customHeight="1">
       <c r="A69" s="5">
         <v>610</v>
       </c>
       <c r="B69" t="s" s="3">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C69" t="s" s="3">
-        <v>115</v>
-      </c>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="7"/>
+        <v>113</v>
+      </c>
+      <c r="D69" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E69" s="7"/>
     </row>
     <row r="70" ht="17" customHeight="1">
       <c r="A70" s="5">
         <v>620</v>
       </c>
       <c r="B70" t="s" s="3">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C70" t="s" s="3">
-        <v>117</v>
-      </c>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="7"/>
+        <v>115</v>
+      </c>
+      <c r="D70" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E70" s="7"/>
     </row>
     <row r="71" ht="17" customHeight="1">
       <c r="A71" s="5">
         <v>630</v>
       </c>
       <c r="B71" t="s" s="3">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C71" t="s" s="3">
-        <v>119</v>
-      </c>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="7"/>
+        <v>117</v>
+      </c>
+      <c r="D71" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E71" s="7"/>
     </row>
     <row r="72" ht="17" customHeight="1">
       <c r="A72" s="5">
         <v>640</v>
       </c>
       <c r="B72" t="s" s="3">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C72" t="s" s="3">
-        <v>121</v>
-      </c>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="7"/>
+        <v>119</v>
+      </c>
+      <c r="D72" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E72" s="7"/>
     </row>
     <row r="73" ht="17" customHeight="1">
       <c r="A73" s="5">
         <v>650</v>
       </c>
       <c r="B73" t="s" s="3">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C73" t="s" s="3">
-        <v>35</v>
-      </c>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="11"/>
+        <v>33</v>
+      </c>
+      <c r="D73" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="E73" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.787402" right="0.787402" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add cardio exercises support.
</commit_message>
<xml_diff>
--- a/src/main/dictionary/Exercises.xlsx
+++ b/src/main/dictionary/Exercises.xlsx
@@ -5,13 +5,15 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" r:id="rId4"/>
+    <sheet name="Strength" sheetId="1" r:id="rId4"/>
+    <sheet name="Cardio" sheetId="2" r:id="rId5"/>
+    <sheet name="Weight Loss" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="134">
   <si>
     <t>id</t>
   </si>
@@ -374,6 +376,45 @@
   </si>
   <si>
     <t>Chin-Ups</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Treadmill</t>
+  </si>
+  <si>
+    <t>Steady Pace Walk or Jog</t>
+  </si>
+  <si>
+    <t>cardio</t>
+  </si>
+  <si>
+    <t>4 x 4 intervals</t>
+  </si>
+  <si>
+    <t>3 x 3 intervals</t>
+  </si>
+  <si>
+    <t>30 second sprints</t>
+  </si>
+  <si>
+    <t>Bike</t>
+  </si>
+  <si>
+    <t>Steady Pace</t>
+  </si>
+  <si>
+    <t>Rowing Machine</t>
+  </si>
+  <si>
+    <t>30 second intervals</t>
+  </si>
+  <si>
+    <t>3 x 3</t>
+  </si>
+  <si>
+    <t>Weight Loss</t>
   </si>
 </sst>
 </file>
@@ -420,7 +461,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -480,13 +521,103 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -523,6 +654,54 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,6 +721,7 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -2679,4 +2859,811 @@
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14" defaultRowHeight="15.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="14" style="12" customWidth="1"/>
+    <col min="2" max="2" width="21.625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="14" style="12" customWidth="1"/>
+    <col min="4" max="4" width="14" style="12" customWidth="1"/>
+    <col min="5" max="5" width="14" style="12" customWidth="1"/>
+    <col min="6" max="256" width="14" style="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="17" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="13">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" ht="16.65" customHeight="1">
+      <c r="A2" s="14">
+        <v>800</v>
+      </c>
+      <c r="B2" t="s" s="15">
+        <v>122</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" ht="16.35" customHeight="1">
+      <c r="A3" s="18">
+        <v>810</v>
+      </c>
+      <c r="B3" t="s" s="19">
+        <v>123</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" t="s" s="19">
+        <v>124</v>
+      </c>
+      <c r="E3" s="17"/>
+    </row>
+    <row r="4" ht="16.35" customHeight="1">
+      <c r="A4" s="18">
+        <v>820</v>
+      </c>
+      <c r="B4" t="s" s="19">
+        <v>125</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" t="s" s="19">
+        <v>124</v>
+      </c>
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" ht="16.35" customHeight="1">
+      <c r="A5" s="18">
+        <v>830</v>
+      </c>
+      <c r="B5" t="s" s="19">
+        <v>126</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" t="s" s="19">
+        <v>124</v>
+      </c>
+      <c r="E5" s="17"/>
+    </row>
+    <row r="6" ht="16.35" customHeight="1">
+      <c r="A6" s="18">
+        <v>840</v>
+      </c>
+      <c r="B6" t="s" s="19">
+        <v>127</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" t="s" s="19">
+        <v>124</v>
+      </c>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" ht="16.35" customHeight="1">
+      <c r="A7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+    </row>
+    <row r="8" ht="16.35" customHeight="1">
+      <c r="A8" s="18">
+        <v>850</v>
+      </c>
+      <c r="B8" t="s" s="20">
+        <v>128</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+    </row>
+    <row r="9" ht="16.35" customHeight="1">
+      <c r="A9" s="18">
+        <v>860</v>
+      </c>
+      <c r="B9" t="s" s="19">
+        <v>129</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" t="s" s="19">
+        <v>124</v>
+      </c>
+      <c r="E9" s="17"/>
+    </row>
+    <row r="10" ht="16.35" customHeight="1">
+      <c r="A10" s="18">
+        <v>870</v>
+      </c>
+      <c r="B10" t="s" s="19">
+        <v>125</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" t="s" s="19">
+        <v>124</v>
+      </c>
+      <c r="E10" s="17"/>
+    </row>
+    <row r="11" ht="16.35" customHeight="1">
+      <c r="A11" s="18">
+        <v>880</v>
+      </c>
+      <c r="B11" t="s" s="19">
+        <v>126</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" t="s" s="19">
+        <v>124</v>
+      </c>
+      <c r="E11" s="17"/>
+    </row>
+    <row r="12" ht="16.35" customHeight="1">
+      <c r="A12" s="18"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+    </row>
+    <row r="13" ht="16.35" customHeight="1">
+      <c r="A13" s="18">
+        <v>890</v>
+      </c>
+      <c r="B13" t="s" s="20">
+        <v>130</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+    </row>
+    <row r="14" ht="16.35" customHeight="1">
+      <c r="A14" s="18">
+        <v>900</v>
+      </c>
+      <c r="B14" t="s" s="19">
+        <v>129</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" t="s" s="19">
+        <v>124</v>
+      </c>
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" ht="16.35" customHeight="1">
+      <c r="A15" s="18">
+        <v>910</v>
+      </c>
+      <c r="B15" t="s" s="19">
+        <v>131</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" t="s" s="19">
+        <v>124</v>
+      </c>
+      <c r="E15" s="17"/>
+    </row>
+    <row r="16" ht="16.35" customHeight="1">
+      <c r="A16" s="18">
+        <v>920</v>
+      </c>
+      <c r="B16" t="s" s="19">
+        <v>132</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" t="s" s="19">
+        <v>124</v>
+      </c>
+      <c r="E16" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14" defaultRowHeight="15.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="14" style="21" customWidth="1"/>
+    <col min="2" max="2" width="21.2031" style="21" customWidth="1"/>
+    <col min="3" max="3" width="18.6016" style="21" customWidth="1"/>
+    <col min="4" max="4" width="14" style="21" customWidth="1"/>
+    <col min="5" max="5" width="14" style="21" customWidth="1"/>
+    <col min="6" max="256" width="14" style="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="17" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="13">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" ht="16.65" customHeight="1">
+      <c r="A2" s="14">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s" s="15">
+        <v>4</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" ht="16.35" customHeight="1">
+      <c r="A3" s="18">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s" s="19">
+        <v>6</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E3" s="17"/>
+    </row>
+    <row r="4" ht="16.35" customHeight="1">
+      <c r="A4" s="18">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s" s="19">
+        <v>9</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" ht="16.35" customHeight="1">
+      <c r="A5" s="18">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s" s="19">
+        <v>11</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E5" s="17"/>
+    </row>
+    <row r="6" ht="16.35" customHeight="1">
+      <c r="A6" s="18">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s" s="19">
+        <v>13</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" ht="16.35" customHeight="1">
+      <c r="A7" s="18">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s" s="19">
+        <v>15</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E7" s="17"/>
+    </row>
+    <row r="8" ht="16.35" customHeight="1">
+      <c r="A8" s="18">
+        <v>120</v>
+      </c>
+      <c r="B8" t="s" s="19">
+        <v>26</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E8" s="17"/>
+    </row>
+    <row r="9" ht="16.35" customHeight="1">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+    </row>
+    <row r="10" ht="16.65" customHeight="1">
+      <c r="A10" s="18">
+        <v>140</v>
+      </c>
+      <c r="B10" t="s" s="22">
+        <v>30</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+    </row>
+    <row r="11" ht="17" customHeight="1">
+      <c r="A11" s="23">
+        <v>170</v>
+      </c>
+      <c r="B11" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E11" s="17"/>
+    </row>
+    <row r="12" ht="17" customHeight="1">
+      <c r="A12" s="23">
+        <v>240</v>
+      </c>
+      <c r="B12" t="s" s="3">
+        <v>44</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E12" s="17"/>
+    </row>
+    <row r="13" ht="17" customHeight="1">
+      <c r="A13" s="23">
+        <v>210</v>
+      </c>
+      <c r="B13" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="C13" s="24"/>
+      <c r="D13" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E13" s="17"/>
+    </row>
+    <row r="14" ht="16.65" customHeight="1">
+      <c r="A14" s="17"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" ht="16.65" customHeight="1">
+      <c r="A15" s="25">
+        <v>250</v>
+      </c>
+      <c r="B15" t="s" s="22">
+        <v>46</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+    </row>
+    <row r="16" ht="17" customHeight="1">
+      <c r="A16" s="5">
+        <v>300</v>
+      </c>
+      <c r="B16" t="s" s="3">
+        <v>56</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E16" s="17"/>
+    </row>
+    <row r="17" ht="17" customHeight="1">
+      <c r="A17" s="5">
+        <v>310</v>
+      </c>
+      <c r="B17" t="s" s="3">
+        <v>58</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E17" s="17"/>
+    </row>
+    <row r="18" ht="17" customHeight="1">
+      <c r="A18" s="5">
+        <v>260</v>
+      </c>
+      <c r="B18" t="s" s="3">
+        <v>48</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E18" s="17"/>
+    </row>
+    <row r="19" ht="17" customHeight="1">
+      <c r="A19" s="5">
+        <v>280</v>
+      </c>
+      <c r="B19" t="s" s="3">
+        <v>52</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E19" s="17"/>
+    </row>
+    <row r="20" ht="16.65" customHeight="1">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+    </row>
+    <row r="21" ht="16.65" customHeight="1">
+      <c r="A21" s="25">
+        <v>330</v>
+      </c>
+      <c r="B21" t="s" s="22">
+        <v>62</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" ht="17" customHeight="1">
+      <c r="A22" s="5">
+        <v>340</v>
+      </c>
+      <c r="B22" t="s" s="3">
+        <v>64</v>
+      </c>
+      <c r="C22" s="24"/>
+      <c r="D22" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E22" s="17"/>
+    </row>
+    <row r="23" ht="17" customHeight="1">
+      <c r="A23" s="5">
+        <v>350</v>
+      </c>
+      <c r="B23" t="s" s="3">
+        <v>66</v>
+      </c>
+      <c r="C23" s="24"/>
+      <c r="D23" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E23" s="17"/>
+    </row>
+    <row r="24" ht="17" customHeight="1">
+      <c r="A24" s="5">
+        <v>400</v>
+      </c>
+      <c r="B24" t="s" s="3">
+        <v>76</v>
+      </c>
+      <c r="C24" s="24"/>
+      <c r="D24" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" ht="17" customHeight="1">
+      <c r="A25" s="5">
+        <v>420</v>
+      </c>
+      <c r="B25" t="s" s="3">
+        <v>44</v>
+      </c>
+      <c r="C25" s="24"/>
+      <c r="D25" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" ht="16.65" customHeight="1">
+      <c r="A26" s="14"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+    </row>
+    <row r="27" ht="16.65" customHeight="1">
+      <c r="A27" s="25">
+        <v>430</v>
+      </c>
+      <c r="B27" t="s" s="22">
+        <v>78</v>
+      </c>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+    </row>
+    <row r="28" ht="17" customHeight="1">
+      <c r="A28" s="5">
+        <v>440</v>
+      </c>
+      <c r="B28" t="s" s="3">
+        <v>80</v>
+      </c>
+      <c r="C28" s="24"/>
+      <c r="D28" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E28" s="17"/>
+    </row>
+    <row r="29" ht="17" customHeight="1">
+      <c r="A29" s="5">
+        <v>450</v>
+      </c>
+      <c r="B29" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="C29" s="24"/>
+      <c r="D29" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E29" s="17"/>
+    </row>
+    <row r="30" ht="17" customHeight="1">
+      <c r="A30" s="5">
+        <v>460</v>
+      </c>
+      <c r="B30" t="s" s="3">
+        <v>84</v>
+      </c>
+      <c r="C30" s="24"/>
+      <c r="D30" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E30" s="17"/>
+    </row>
+    <row r="31" ht="17" customHeight="1">
+      <c r="A31" s="5">
+        <v>470</v>
+      </c>
+      <c r="B31" t="s" s="3">
+        <v>86</v>
+      </c>
+      <c r="C31" s="24"/>
+      <c r="D31" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E31" s="17"/>
+    </row>
+    <row r="32" ht="17" customHeight="1">
+      <c r="A32" s="5"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+    </row>
+    <row r="33" ht="17" customHeight="1">
+      <c r="A33" s="26">
+        <v>800</v>
+      </c>
+      <c r="B33" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="C33" s="24"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+    </row>
+    <row r="34" ht="16.65" customHeight="1">
+      <c r="A34" s="18">
+        <v>810</v>
+      </c>
+      <c r="B34" t="s" s="27">
+        <v>123</v>
+      </c>
+      <c r="C34" s="17"/>
+      <c r="D34" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E34" s="17"/>
+    </row>
+    <row r="35" ht="16.35" customHeight="1">
+      <c r="A35" s="18">
+        <v>820</v>
+      </c>
+      <c r="B35" t="s" s="19">
+        <v>125</v>
+      </c>
+      <c r="C35" s="17"/>
+      <c r="D35" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E35" s="17"/>
+    </row>
+    <row r="36" ht="16.35" customHeight="1">
+      <c r="A36" s="18">
+        <v>830</v>
+      </c>
+      <c r="B36" t="s" s="19">
+        <v>126</v>
+      </c>
+      <c r="C36" s="17"/>
+      <c r="D36" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E36" s="17"/>
+    </row>
+    <row r="37" ht="16.35" customHeight="1">
+      <c r="A37" s="18">
+        <v>840</v>
+      </c>
+      <c r="B37" t="s" s="19">
+        <v>127</v>
+      </c>
+      <c r="C37" s="17"/>
+      <c r="D37" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E37" s="17"/>
+    </row>
+    <row r="38" ht="16.35" customHeight="1">
+      <c r="A38" s="18"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+    </row>
+    <row r="39" ht="16.35" customHeight="1">
+      <c r="A39" s="18">
+        <v>850</v>
+      </c>
+      <c r="B39" t="s" s="20">
+        <v>128</v>
+      </c>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+    </row>
+    <row r="40" ht="16.35" customHeight="1">
+      <c r="A40" s="18">
+        <v>860</v>
+      </c>
+      <c r="B40" t="s" s="19">
+        <v>129</v>
+      </c>
+      <c r="C40" s="17"/>
+      <c r="D40" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E40" s="17"/>
+    </row>
+    <row r="41" ht="16.35" customHeight="1">
+      <c r="A41" s="18">
+        <v>870</v>
+      </c>
+      <c r="B41" t="s" s="19">
+        <v>125</v>
+      </c>
+      <c r="C41" s="17"/>
+      <c r="D41" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E41" s="17"/>
+    </row>
+    <row r="42" ht="16.35" customHeight="1">
+      <c r="A42" s="18">
+        <v>880</v>
+      </c>
+      <c r="B42" t="s" s="19">
+        <v>126</v>
+      </c>
+      <c r="C42" s="17"/>
+      <c r="D42" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E42" s="17"/>
+    </row>
+    <row r="43" ht="16.35" customHeight="1">
+      <c r="A43" s="18"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+    </row>
+    <row r="44" ht="16.35" customHeight="1">
+      <c r="A44" s="18">
+        <v>890</v>
+      </c>
+      <c r="B44" t="s" s="20">
+        <v>130</v>
+      </c>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+    </row>
+    <row r="45" ht="16.35" customHeight="1">
+      <c r="A45" s="18">
+        <v>900</v>
+      </c>
+      <c r="B45" t="s" s="19">
+        <v>129</v>
+      </c>
+      <c r="C45" s="17"/>
+      <c r="D45" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E45" s="17"/>
+    </row>
+    <row r="46" ht="16.35" customHeight="1">
+      <c r="A46" s="18">
+        <v>910</v>
+      </c>
+      <c r="B46" t="s" s="19">
+        <v>131</v>
+      </c>
+      <c r="C46" s="17"/>
+      <c r="D46" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E46" s="17"/>
+    </row>
+    <row r="47" ht="16.35" customHeight="1">
+      <c r="A47" s="18">
+        <v>920</v>
+      </c>
+      <c r="B47" t="s" s="19">
+        <v>132</v>
+      </c>
+      <c r="C47" s="17"/>
+      <c r="D47" t="s" s="19">
+        <v>133</v>
+      </c>
+      <c r="E47" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>